<commit_message>
Netzplanübung 2 - Lösung Tabelle 1
</commit_message>
<xml_diff>
--- a/Übungen/03_Netzplan_Übung2.xlsx
+++ b/Übungen/03_Netzplan_Übung2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -358,7 +358,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -366,7 +366,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,19 +390,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +564,7 @@
   <dimension ref="A1:AJ32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
+      <selection pane="topLeft" activeCell="R16" activeCellId="0" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -661,9 +661,15 @@
       <c r="P2" s="0"/>
       <c r="Q2" s="0"/>
       <c r="R2" s="0"/>
-      <c r="U2" s="7"/>
+      <c r="U2" s="7" t="n">
+        <f aca="false">R8</f>
+        <v>20</v>
+      </c>
       <c r="V2" s="8"/>
-      <c r="W2" s="9"/>
+      <c r="W2" s="9" t="n">
+        <f aca="false">U2+U4</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -753,8 +759,14 @@
         <f aca="false">VLOOKUP(U3,$A$2:$K$9,11)</f>
         <v>11</v>
       </c>
-      <c r="V4" s="15"/>
-      <c r="W4" s="16"/>
+      <c r="V4" s="15" t="n">
+        <f aca="false">W5-W2</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="16" t="n">
+        <f aca="false">AE8-W2</f>
+        <v>0</v>
+      </c>
       <c r="Y4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,9 +804,15 @@
       <c r="Q5" s="0"/>
       <c r="R5" s="0"/>
       <c r="T5" s="13"/>
-      <c r="U5" s="17"/>
+      <c r="U5" s="17" t="n">
+        <f aca="false">W5-U4</f>
+        <v>20</v>
+      </c>
       <c r="V5" s="8"/>
-      <c r="W5" s="18"/>
+      <c r="W5" s="18" t="n">
+        <f aca="false">AE11</f>
+        <v>31</v>
+      </c>
       <c r="Y5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,23 +924,41 @@
         <f aca="false">ROUNDUP(H8/(I8*J8),0)</f>
         <v>4</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="P8" s="7" t="n">
+        <f aca="false">M11</f>
+        <v>12</v>
+      </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="9"/>
+      <c r="R8" s="9" t="n">
+        <f aca="false">P8+P10</f>
+        <v>20</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="13"/>
-      <c r="U8" s="7"/>
+      <c r="U8" s="7" t="n">
+        <f aca="false">R8</f>
+        <v>20</v>
+      </c>
       <c r="V8" s="8"/>
-      <c r="W8" s="9"/>
+      <c r="W8" s="9" t="n">
+        <f aca="false">U8+U10</f>
+        <v>26</v>
+      </c>
       <c r="Y8" s="19"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
-      <c r="AE8" s="7"/>
+      <c r="AE8" s="7" t="n">
+        <f aca="false">MAX(W2,W14,AB20)</f>
+        <v>31</v>
+      </c>
       <c r="AF8" s="8"/>
-      <c r="AG8" s="9"/>
+      <c r="AG8" s="9" t="n">
+        <f aca="false">AE8+AE10</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
@@ -984,15 +1020,27 @@
         <f aca="false">VLOOKUP(P9,$A$2:$K$9,11)</f>
         <v>8</v>
       </c>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="16"/>
+      <c r="Q10" s="15" t="n">
+        <f aca="false">R11-R8</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="16" t="n">
+        <f aca="false">MIN(U2,U8,U14)-R8</f>
+        <v>0</v>
+      </c>
       <c r="S10" s="10"/>
       <c r="U10" s="14" t="n">
         <f aca="false">VLOOKUP(U9,$A$2:$K$9,11)</f>
         <v>6</v>
       </c>
-      <c r="V10" s="15"/>
-      <c r="W10" s="16"/>
+      <c r="V10" s="15" t="n">
+        <f aca="false">W11-W8</f>
+        <v>1</v>
+      </c>
+      <c r="W10" s="16" t="n">
+        <f aca="false">Z20-W8</f>
+        <v>0</v>
+      </c>
       <c r="X10" s="0"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="25"/>
@@ -1004,8 +1052,13 @@
         <f aca="false">VLOOKUP(AE9,$A$2:$K$9,11)</f>
         <v>2</v>
       </c>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="16"/>
+      <c r="AF10" s="15" t="n">
+        <f aca="false">AG11-AG8</f>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
@@ -1019,22 +1072,43 @@
         <v>0</v>
       </c>
       <c r="L11" s="8"/>
-      <c r="M11" s="9"/>
+      <c r="M11" s="9" t="n">
+        <f aca="false">K11+K13</f>
+        <v>12</v>
+      </c>
       <c r="N11" s="10"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="17"/>
+      <c r="P11" s="17" t="n">
+        <f aca="false">R11-P10</f>
+        <v>12</v>
+      </c>
       <c r="Q11" s="8"/>
-      <c r="R11" s="18"/>
+      <c r="R11" s="18" t="n">
+        <f aca="false">MIN(U5,U11,U17)</f>
+        <v>20</v>
+      </c>
       <c r="T11" s="13"/>
-      <c r="U11" s="17"/>
+      <c r="U11" s="17" t="n">
+        <f aca="false">W11-U10</f>
+        <v>21</v>
+      </c>
       <c r="V11" s="8"/>
-      <c r="W11" s="18"/>
+      <c r="W11" s="18" t="n">
+        <f aca="false">Z23</f>
+        <v>27</v>
+      </c>
       <c r="Y11" s="13"/>
       <c r="Z11" s="25"/>
       <c r="AD11" s="13"/>
-      <c r="AE11" s="17"/>
+      <c r="AE11" s="17" t="n">
+        <f aca="false">AG11-AE10</f>
+        <v>31</v>
+      </c>
       <c r="AF11" s="8"/>
-      <c r="AG11" s="18"/>
+      <c r="AG11" s="18" t="n">
+        <f aca="false">AG8</f>
+        <v>33</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
@@ -1090,17 +1164,35 @@
       <c r="C14" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="17" t="n">
+        <f aca="false">M14-K13</f>
+        <v>0</v>
+      </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="18"/>
+      <c r="M14" s="18" t="n">
+        <f aca="false">MIN(P11,P17)</f>
+        <v>12</v>
+      </c>
       <c r="O14" s="13"/>
-      <c r="P14" s="7"/>
+      <c r="P14" s="7" t="n">
+        <f aca="false">M11</f>
+        <v>12</v>
+      </c>
       <c r="Q14" s="8"/>
-      <c r="R14" s="9"/>
+      <c r="R14" s="9" t="n">
+        <f aca="false">P14+P16</f>
+        <v>18</v>
+      </c>
       <c r="T14" s="19"/>
-      <c r="U14" s="7"/>
+      <c r="U14" s="7" t="n">
+        <f aca="false">MAX(R8,R14)</f>
+        <v>20</v>
+      </c>
       <c r="V14" s="8"/>
-      <c r="W14" s="9"/>
+      <c r="W14" s="9" t="n">
+        <f aca="false">U14+U16</f>
+        <v>27</v>
+      </c>
       <c r="Y14" s="13"/>
       <c r="Z14" s="25"/>
       <c r="AD14" s="13"/>
@@ -1129,26 +1221,50 @@
         <f aca="false">VLOOKUP(P15,$A$2:$K$9,11)</f>
         <v>6</v>
       </c>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="16"/>
+      <c r="Q16" s="15" t="n">
+        <f aca="false">R17-R14</f>
+        <v>6</v>
+      </c>
+      <c r="R16" s="16" t="n">
+        <f aca="false">MIN(U14,Z20)-R14</f>
+        <v>2</v>
+      </c>
       <c r="S16" s="10"/>
       <c r="U16" s="14" t="n">
         <f aca="false">VLOOKUP(U15,$A$2:$K$9,11)</f>
         <v>7</v>
       </c>
-      <c r="V16" s="15"/>
-      <c r="W16" s="16"/>
+      <c r="V16" s="15" t="n">
+        <f aca="false">W17-W14</f>
+        <v>4</v>
+      </c>
+      <c r="W16" s="16" t="n">
+        <f aca="false">AE8-W14</f>
+        <v>4</v>
+      </c>
       <c r="Y16" s="13"/>
       <c r="AD16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P17" s="17"/>
+      <c r="P17" s="17" t="n">
+        <f aca="false">R17-P16</f>
+        <v>18</v>
+      </c>
       <c r="Q17" s="8"/>
-      <c r="R17" s="18"/>
+      <c r="R17" s="18" t="n">
+        <f aca="false">MIN(U17,Z23)</f>
+        <v>24</v>
+      </c>
       <c r="T17" s="13"/>
-      <c r="U17" s="17"/>
+      <c r="U17" s="17" t="n">
+        <f aca="false">W17-U16</f>
+        <v>24</v>
+      </c>
       <c r="V17" s="8"/>
-      <c r="W17" s="18"/>
+      <c r="W17" s="18" t="n">
+        <f aca="false">AE11</f>
+        <v>31</v>
+      </c>
       <c r="Y17" s="13"/>
       <c r="AD17" s="13"/>
     </row>
@@ -1168,9 +1284,15 @@
       <c r="V20" s="0"/>
       <c r="W20" s="0"/>
       <c r="Y20" s="19"/>
-      <c r="Z20" s="7"/>
+      <c r="Z20" s="7" t="n">
+        <f aca="false">MAX(W8,R14)</f>
+        <v>26</v>
+      </c>
       <c r="AA20" s="8"/>
-      <c r="AB20" s="9"/>
+      <c r="AB20" s="9" t="n">
+        <f aca="false">Z20+Z22</f>
+        <v>30</v>
+      </c>
       <c r="AD20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,16 +1318,28 @@
         <f aca="false">VLOOKUP(Z21,$A$2:$K$9,11)</f>
         <v>4</v>
       </c>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="16"/>
+      <c r="AA22" s="15" t="n">
+        <f aca="false">AB23-AB20</f>
+        <v>1</v>
+      </c>
+      <c r="AB22" s="16" t="n">
+        <f aca="false">AE8-AB20</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="U23" s="0"/>
       <c r="V23" s="0"/>
       <c r="W23" s="0"/>
-      <c r="Z23" s="17"/>
+      <c r="Z23" s="17" t="n">
+        <f aca="false">AB23-Z22</f>
+        <v>27</v>
+      </c>
       <c r="AA23" s="8"/>
-      <c r="AB23" s="18"/>
+      <c r="AB23" s="18" t="n">
+        <f aca="false">AE11</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A25" s="28" t="s">
@@ -1298,7 +1432,7 @@
     <mergeCell ref="Z21:AB21"/>
     <mergeCell ref="A25:G25"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF10 AA22 V16 V10 V4 Q16 Q10 L13">
+  <conditionalFormatting sqref="AF10 L13 AA22 V16 V10 V4 Q10 Q16">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -1320,8 +1454,8 @@
   </sheetPr>
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P23" activeCellId="0" sqref="P23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V21" activeCellId="0" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2134,8 +2268,8 @@
   </sheetPr>
   <dimension ref="A1:AH23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V18" activeCellId="0" sqref="V18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>